<commit_message>
Use new basic formula support
</commit_message>
<xml_diff>
--- a/resources/portfolio-template.xlsx
+++ b/resources/portfolio-template.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16340" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="0" windowWidth="25720" windowHeight="8660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Portfolio" sheetId="1" r:id="rId1"/>
@@ -197,17 +197,7 @@
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -551,7 +541,7 @@
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -667,7 +657,8 @@
         <v>3.82</v>
       </c>
       <c r="H5" s="5">
-        <v>12000</v>
+        <f>B5*G5</f>
+        <v>764</v>
       </c>
       <c r="I5" s="12"/>
       <c r="J5" s="5">
@@ -683,17 +674,21 @@
         <v>3.82</v>
       </c>
       <c r="N5" s="5">
-        <v>12000</v>
+        <f>B5*M5</f>
+        <v>764</v>
       </c>
       <c r="O5" s="11"/>
       <c r="P5" s="5">
-        <v>0.12</v>
+        <f>M5-G5</f>
+        <v>0</v>
       </c>
       <c r="Q5" s="5">
-        <v>63.5</v>
+        <f>N5-H5</f>
+        <v>0</v>
       </c>
       <c r="R5" s="9">
-        <v>2.3E-2</v>
+        <f>Q5/H5</f>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:18">
@@ -706,7 +701,8 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="14">
-        <v>15000</v>
+        <f>SUM(H5:H5)</f>
+        <v>764</v>
       </c>
       <c r="I6" s="12"/>
       <c r="J6" s="3"/>
@@ -714,20 +710,23 @@
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
       <c r="N6" s="14">
-        <v>15000</v>
+        <f>SUM(N5:N5)</f>
+        <v>764</v>
       </c>
       <c r="O6" s="11"/>
       <c r="P6" s="3"/>
       <c r="Q6" s="14">
-        <v>790</v>
+        <f>N6-H6</f>
+        <v>0</v>
       </c>
       <c r="R6" s="15">
-        <v>1.2E-2</v>
+        <f>Q6/H6</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="P1:R1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Add a pie chart!
</commit_message>
<xml_diff>
--- a/resources/portfolio-template.xlsx
+++ b/resources/portfolio-template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="0" windowWidth="25720" windowHeight="8660" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="13980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Portfolio" sheetId="1" r:id="rId1"/>
@@ -213,6 +213,128 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Allocation</c:v>
+          </c:tx>
+          <c:dLbls>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Portfolio!$A$5:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MSFT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Portfolio!$N$5:$N$5</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>764.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>6</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>76206</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -541,7 +663,7 @@
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -732,6 +854,7 @@
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
WIP on adding per-stock history to the spreadsheet
</commit_message>
<xml_diff>
--- a/resources/portfolio-template.xlsx
+++ b/resources/portfolio-template.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="13980" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15260" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Portfolio" sheetId="1" r:id="rId1"/>
+    <sheet name="PerStock" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>Stock</t>
   </si>
@@ -67,13 +68,31 @@
   </si>
   <si>
     <t>Portfolio Status as of February 2, 2015</t>
+  </si>
+  <si>
+    <t>YTD Info for Stock</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Ticker</t>
+  </si>
+  <si>
+    <t>Holdings:</t>
+  </si>
+  <si>
+    <t>Value</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="mmm\ dd;@"/>
+  </numFmts>
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -124,6 +143,19 @@
       <color theme="1"/>
       <name val="e"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -168,7 +200,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -185,6 +217,15 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -300,6 +341,124 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Value</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>PerStock!$A$5:$A$5</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\ dd;@</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>42006.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>PerStock!$D$5:$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1.25919E6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2080480712"/>
+        <c:axId val="-2080479304"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="-2080480712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="mmm\ dd;@" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2080479304"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="-2080479304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2080480712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -318,6 +477,41 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -659,7 +853,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
@@ -861,4 +1055,79 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="17" customFormat="1" ht="20">
+      <c r="A1" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="16"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="19">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="22">
+        <v>42006</v>
+      </c>
+      <c r="B5" s="21">
+        <v>98</v>
+      </c>
+      <c r="C5" s="21">
+        <v>102</v>
+      </c>
+      <c r="D5" s="20">
+        <f>C5*$C$2</f>
+        <v>1259190</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added ranges and formulas
</commit_message>
<xml_diff>
--- a/resources/portfolio-template.xlsx
+++ b/resources/portfolio-template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15260" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-20" yWindow="0" windowWidth="28900" windowHeight="15260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Portfolio" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>Stock</t>
   </si>
@@ -83,6 +83,12 @@
   </si>
   <si>
     <t>Value</t>
+  </si>
+  <si>
+    <t>Daily Change</t>
+  </si>
+  <si>
+    <t>YTD Change</t>
   </si>
 </sst>
 </file>
@@ -90,7 +96,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="mmm\ dd;@"/>
+    <numFmt numFmtId="164" formatCode="mmm\ dd;@"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -225,7 +231,7 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -341,124 +347,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Value</c:v>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>PerStock!$A$5:$A$5</c:f>
-              <c:numCache>
-                <c:formatCode>mmm\ dd;@</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>42006.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>PerStock!$D$5:$D$5</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0.00</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>1.25919E6</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="-2080480712"/>
-        <c:axId val="-2080479304"/>
-      </c:lineChart>
-      <c:dateAx>
-        <c:axId val="-2080480712"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="mmm\ dd;@" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2080479304"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
-      <c:valAx>
-        <c:axId val="-2080479304"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2080480712"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -477,41 +365,6 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Chart 2"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -853,11 +706,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="R14" sqref="R14"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1059,24 +912,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="17" customFormat="1" ht="20">
+    <row r="1" spans="1:6" s="17" customFormat="1" ht="20">
       <c r="A1" s="16" t="s">
         <v>16</v>
       </c>
       <c r="C1" s="16"/>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
@@ -1086,13 +941,17 @@
       <c r="C2" s="19">
         <v>12345</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="2"/>
       <c r="B3" s="18"/>
       <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
@@ -1103,10 +962,16 @@
         <v>7</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:6">
       <c r="A5" s="22">
         <v>42006</v>
       </c>
@@ -1116,14 +981,38 @@
       <c r="C5" s="21">
         <v>102</v>
       </c>
-      <c r="D5" s="20">
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="20">
         <f>C5*$C$2</f>
         <v>1259190</v>
       </c>
     </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="22">
+        <v>42007</v>
+      </c>
+      <c r="B6" s="21">
+        <v>98</v>
+      </c>
+      <c r="C6" s="21">
+        <v>102</v>
+      </c>
+      <c r="D6" s="21">
+        <f>C6-C5</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="21">
+        <f>C6-$B$5</f>
+        <v>4</v>
+      </c>
+      <c r="F6" s="20">
+        <f>C6*$C$2</f>
+        <v>1259190</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Added the combined history chart
</commit_message>
<xml_diff>
--- a/resources/portfolio-template.xlsx
+++ b/resources/portfolio-template.xlsx
@@ -4,11 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="0" windowWidth="28900" windowHeight="15260" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Portfolio" sheetId="1" r:id="rId1"/>
-    <sheet name="PerStock" sheetId="2" r:id="rId2"/>
+    <sheet name="Allocation" sheetId="5" r:id="rId2"/>
+    <sheet name="Performance" sheetId="6" r:id="rId3"/>
+    <sheet name="PerStock" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <t>Stock</t>
   </si>
@@ -89,6 +91,9 @@
   </si>
   <si>
     <t>YTD Change</t>
+  </si>
+  <si>
+    <t>YTD Pct Change</t>
   </si>
 </sst>
 </file>
@@ -347,6 +352,262 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Allocation</c:v>
+          </c:tx>
+          <c:dLbls>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Portfolio!$A$5:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MSFT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Portfolio!$N$5:$N$5</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>764.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Relative</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Performance</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>PerStock!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ticker</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>PerStock!$A$5:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\ dd;@</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>42006.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42007.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>PerStock!$F$5:$F$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1.040816326530612</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.040816326530612</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2142116664"/>
+        <c:axId val="2143479304"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="2142116664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="mmm\ dd;@" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2143479304"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="2143479304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2142116664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="132" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="132" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -379,6 +640,60 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8582121" cy="5830455"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8582121" cy="5830455"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
 </xdr:wsDr>
 </file>
 
@@ -706,11 +1021,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="S25" sqref="S25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -912,26 +1227,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="4" max="6" width="12.33203125" customWidth="1"/>
+    <col min="4" max="7" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="17" customFormat="1" ht="20">
+    <row r="1" spans="1:7" s="17" customFormat="1" ht="20">
       <c r="A1" s="16" t="s">
         <v>16</v>
       </c>
       <c r="C1" s="16"/>
       <c r="D1" s="16"/>
       <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
@@ -943,15 +1257,17 @@
       </c>
       <c r="D2" s="19"/>
       <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" s="2"/>
       <c r="B3" s="18"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
@@ -968,10 +1284,13 @@
         <v>22</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5" s="22">
         <v>42006</v>
       </c>
@@ -983,12 +1302,16 @@
       </c>
       <c r="D5" s="21"/>
       <c r="E5" s="21"/>
-      <c r="F5" s="20">
+      <c r="F5" s="21">
+        <f>C5/$B$5</f>
+        <v>1.0408163265306123</v>
+      </c>
+      <c r="G5" s="20">
         <f>C5*$C$2</f>
         <v>1259190</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7">
       <c r="A6" s="22">
         <v>42007</v>
       </c>
@@ -1006,7 +1329,11 @@
         <f>C6-$B$5</f>
         <v>4</v>
       </c>
-      <c r="F6" s="20">
+      <c r="F6" s="21">
+        <f>C6/$B$5</f>
+        <v>1.0408163265306123</v>
+      </c>
+      <c r="G6" s="20">
         <f>C6*$C$2</f>
         <v>1259190</v>
       </c>

</xml_diff>

<commit_message>
Remove the date conversion now that it's built into excel-templates
</commit_message>
<xml_diff>
--- a/resources/portfolio-template.xlsx
+++ b/resources/portfolio-template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Portfolio" sheetId="1" r:id="rId1"/>
@@ -1021,11 +1021,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="S25" sqref="S25"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1229,7 +1229,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>

</xml_diff>

<commit_message>
Strip things down to prep for the demo
</commit_message>
<xml_diff>
--- a/resources/portfolio-template.xlsx
+++ b/resources/portfolio-template.xlsx
@@ -8,9 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="Portfolio" sheetId="1" r:id="rId1"/>
-    <sheet name="Allocation" sheetId="5" r:id="rId2"/>
-    <sheet name="Performance" sheetId="6" r:id="rId3"/>
-    <sheet name="PerStock" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Stock</t>
   </si>
@@ -70,40 +67,13 @@
   </si>
   <si>
     <t>Portfolio Status as of February 2, 2015</t>
-  </si>
-  <si>
-    <t>YTD Info for Stock</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Ticker</t>
-  </si>
-  <si>
-    <t>Holdings:</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>Daily Change</t>
-  </si>
-  <si>
-    <t>YTD Change</t>
-  </si>
-  <si>
-    <t>YTD Pct Change</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="mmm\ dd;@"/>
-  </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -154,19 +124,6 @@
       <color theme="1"/>
       <name val="e"/>
     </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -211,7 +168,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -228,15 +185,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -352,262 +300,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:pieChart>
-        <c:varyColors val="1"/>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Allocation</c:v>
-          </c:tx>
-          <c:dLbls>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="1"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="1"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="1"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Portfolio!$A$5:$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>MSFT</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Portfolio!$N$5:$N$5</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0.00</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>764.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
-        </c:dLbls>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Relative</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Performance</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>PerStock!$A$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Ticker</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>PerStock!$A$5:$A$6</c:f>
-              <c:numCache>
-                <c:formatCode>mmm\ dd;@</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>42006.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>42007.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>PerStock!$F$5:$F$6</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>1.040816326530612</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.040816326530612</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="2142116664"/>
-        <c:axId val="2143479304"/>
-      </c:lineChart>
-      <c:dateAx>
-        <c:axId val="2142116664"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="mmm\ dd;@" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2143479304"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
-      <c:valAx>
-        <c:axId val="2143479304"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142116664"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-</c:chartSpace>
-</file>
-
-<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr/>
-  <sheetViews>
-    <sheetView zoomScale="132" workbookViewId="0" zoomToFit="1"/>
-  </sheetViews>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing r:id="rId1"/>
-</chartsheet>
-</file>
-
-<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr/>
-  <sheetViews>
-    <sheetView zoomScale="132" workbookViewId="0" zoomToFit="1"/>
-  </sheetViews>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing r:id="rId1"/>
-</chartsheet>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -640,60 +332,6 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:absoluteAnchor>
-    <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8582121" cy="5830455"/>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks noGrp="1"/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:absoluteAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:absoluteAnchor>
-    <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8582121" cy="5830455"/>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks noGrp="1"/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:absoluteAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1025,7 +663,7 @@
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1223,130 +861,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="4" max="7" width="12.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" s="17" customFormat="1" ht="20">
-      <c r="A1" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="19">
-        <v>12345</v>
-      </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="2"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="22">
-        <v>42006</v>
-      </c>
-      <c r="B5" s="21">
-        <v>98</v>
-      </c>
-      <c r="C5" s="21">
-        <v>102</v>
-      </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21">
-        <f>C5/$B$5</f>
-        <v>1.0408163265306123</v>
-      </c>
-      <c r="G5" s="20">
-        <f>C5*$C$2</f>
-        <v>1259190</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="22">
-        <v>42007</v>
-      </c>
-      <c r="B6" s="21">
-        <v>98</v>
-      </c>
-      <c r="C6" s="21">
-        <v>102</v>
-      </c>
-      <c r="D6" s="21">
-        <f>C6-C5</f>
-        <v>0</v>
-      </c>
-      <c r="E6" s="21">
-        <f>C6-$B$5</f>
-        <v>4</v>
-      </c>
-      <c r="F6" s="21">
-        <f>C6/$B$5</f>
-        <v>1.0408163265306123</v>
-      </c>
-      <c r="G6" s="20">
-        <f>C6*$C$2</f>
-        <v>1259190</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Crazy zoom for conference
</commit_message>
<xml_diff>
--- a/resources/portfolio-template.xlsx
+++ b/resources/portfolio-template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15960" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Portfolio" sheetId="1" r:id="rId1"/>
@@ -659,11 +659,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" zoomScalePageLayoutView="250" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Added a chart to the PerStock page now that we can clone charts
</commit_message>
<xml_diff>
--- a/resources/portfolio-template.xlsx
+++ b/resources/portfolio-template.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33720" windowHeight="14280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Portfolio" sheetId="1" r:id="rId1"/>
@@ -367,7 +367,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -469,7 +468,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -537,11 +535,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2142116664"/>
-        <c:axId val="2143479304"/>
+        <c:axId val="-2147215512"/>
+        <c:axId val="-2147212488"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2142116664"/>
+        <c:axId val="-2147215512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -551,14 +549,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2143479304"/>
+        <c:crossAx val="-2147212488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2143479304"/>
+        <c:axId val="-2147212488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -569,14 +567,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142116664"/>
+        <c:crossAx val="-2147215512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -586,11 +583,143 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>PerStock!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ticker</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>PerStock!$A$5:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\ dd;@</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>42006.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42007.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>PerStock!$C$5:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>102.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>102.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2141712088"/>
+        <c:axId val="2141715112"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="2141712088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="mmm\ dd;@" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2141715112"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="2141715112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2141712088"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="132" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="187" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -601,7 +730,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="132" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="187" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -647,7 +776,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8582121" cy="5830455"/>
+    <xdr:ext cx="8577594" cy="5833850"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -674,7 +803,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8582121" cy="5830455"/>
+    <xdr:ext cx="8577594" cy="5833850"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -694,6 +823,41 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1231,7 +1395,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="C7" activeCellId="6" sqref="A4:A6 C4 C5 C7 C7 C6 C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1343,6 +1507,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>